<commit_message>
Se agregan algunos nuevos campos
Se agregan algunos campos para mejorar los documentos, estos por ejemplos poner un titulo a las empresas.
</commit_message>
<xml_diff>
--- a/PowerBi/Relleno de Ejemplo/Relleno.xlsx
+++ b/PowerBi/Relleno de Ejemplo/Relleno.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendrik\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DE448A-9DD7-471B-8BBE-326FA866B9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101EC994-03FC-4CB6-A637-0B98FE6A4B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="4" xr2:uid="{FAD7DA82-6D1B-476F-A0CE-7EA27333F172}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{FAD7DA82-6D1B-476F-A0CE-7EA27333F172}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla R_Transacciones" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Tabla Pag_Revisado" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Tabla Pag_Revisado'!$A$1:$D$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tabla R_Transacciones'!$A$1:$D$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>ID_Transacción</t>
   </si>
@@ -175,6 +176,69 @@
   </si>
   <si>
     <t>región</t>
+  </si>
+  <si>
+    <t>Extracciones Mineras del Este, S</t>
+  </si>
+  <si>
+    <t>Corporación de Extracción de Hierro, S</t>
+  </si>
+  <si>
+    <t>Compañía de Minería de Níquel, S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sociedad de Minería de Diamantes, S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compañía de Extracción de Esmeraldas, S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corporación de Minería de Zafiro, S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sociedad Minera de Topacio, S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compañía Minera de Jade, S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corporación Minera de Ópalo, S</t>
+  </si>
+  <si>
+    <t>Minerales y Metales del Norte, SA</t>
+  </si>
+  <si>
+    <t>Exploraciones Geológicas del Sur, SA</t>
+  </si>
+  <si>
+    <t>Compañía Minera de Cobre y Oro, SA</t>
+  </si>
+  <si>
+    <t>Sociedad Minera de Plata y Zinc, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Extracciones de Platino del Oeste, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corporación Minera de Grafito, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sociedad Minera de Rubíes, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compañía de Extracción de Amatista, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corporación de Extracción de Turquesa, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sociedad de Minería de Ámbar, SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Compañía de Extracción de Lapislázuli, SA</t>
+  </si>
+  <si>
+    <t>Nombre_Empresa</t>
   </si>
 </sst>
 </file>
@@ -545,7 +609,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,6 +1336,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D51" xr:uid="{8299C4EC-D1F3-4B09-A9E8-3646892743B9}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1450,7 +1515,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,50 +1695,62 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8491782-EE84-483D-A6A9-61D835E4994C}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>21</v>
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(0,16)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>22</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B21" ca="1" si="0">RANDBETWEEN(0,16)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>23</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>24</v>
       </c>
@@ -1681,149 +1758,201 @@
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>26</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>27</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>28</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>29</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>30</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>31</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>32</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>33</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>34</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>35</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>36</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>37</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>38</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>39</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>40</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +2012,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(0,16)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(0,4)</f>
@@ -1891,7 +2020,7 @@
       </c>
       <c r="F2">
         <f ca="1">RANDBETWEEN(0,16)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1909,19 +2038,19 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C11" ca="1" si="0">RANDBETWEEN(0,4)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D11" ca="1" si="1">RANDBETWEEN(0,36)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E11" ca="1" si="2">RANDBETWEEN(0,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F11" ca="1" si="3">RANDBETWEEN(0,16)</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1947,11 +2076,11 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1973,15 +2102,15 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1999,19 +2128,19 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -2029,11 +2158,11 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="2"/>
@@ -2041,7 +2170,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -2059,19 +2188,19 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -2089,19 +2218,19 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -2123,15 +2252,15 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -2149,19 +2278,19 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -2180,10 +2309,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1702F0F6-1DB7-44FA-AD30-174544B9F3A5}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2321,7 @@
     <col min="2" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2206,7 +2335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2220,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
@@ -2234,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -2248,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>18</v>
       </c>
@@ -2262,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>23</v>
       </c>
@@ -2276,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>28</v>
       </c>
@@ -2290,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>33</v>
       </c>
@@ -2304,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>38</v>
       </c>
@@ -2318,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>43</v>
       </c>
@@ -2332,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>48</v>
       </c>
@@ -2346,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2354,13 +2483,13 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2368,13 +2497,13 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -2382,13 +2511,13 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -2396,13 +2525,13 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>25</v>
       </c>
@@ -2410,11 +2539,12 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -2424,7 +2554,7 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2438,7 +2568,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2452,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2466,7 +2596,7 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -2480,7 +2610,7 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2488,5 +2618,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>